<commit_message>
Removed two files and cleaned up stoch
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ZZ_TIMESReportpy.xlsx
+++ b/SuppXLS/Scen_ZZ_TIMESReportpy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_01\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B103E80-5385-4B12-9EE4-73A28C3B5D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55106B-1C3E-47C3-9EF2-0B4B3DBF4BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,13 +356,13 @@
     <t>TFM_INS</t>
   </si>
   <si>
-    <t>C:\Users\lucas\Desktop\KandidatPyt\FindStats.py</t>
-  </si>
-  <si>
     <t>Filename</t>
   </si>
   <si>
     <t>C:\veda\GAMS_WrkTIMES\%$case_name%\%$case_name%.lst</t>
+  </si>
+  <si>
+    <t>C:\Users\lucas\Documents\KandidatPyt\FindStats.py</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,7 +956,7 @@
       </c>
       <c r="C5" s="10" t="str">
         <f>C14 &amp;" "&amp;C15</f>
-        <v>python C:\Users\lucas\Desktop\KandidatPyt\FindStats.py C:\veda\GAMS_WrkTIMES\%$case_name%\%$case_name%.lst</v>
+        <v>Python C:\Users\lucas\Documents\KandidatPyt\FindStats.py C:\veda\GAMS_WrkTIMES\%$case_name%\%$case_name%.lst</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -971,7 +971,7 @@
       </c>
       <c r="C12" t="str">
         <f ca="1">CELL("filename",$A$1)</f>
-        <v>C:\VEDA\VEDA_models\KModel_01\SuppXLS\[Scen_ZZ_TIMESReportpy.xlsx]RunTIMESReportScript</v>
+        <v>C:\VEDA\Veda_models\KModel_04\SuppXLS\[Scen_ZZ_TIMESReportpy.xlsx]RunTIMESReportScript</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -987,16 +987,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="str">
-        <f>"python "&amp;C13</f>
-        <v>python C:\Users\lucas\Desktop\KandidatPyt\FindStats.py</v>
+        <f>"Python "&amp;C13</f>
+        <v>Python C:\Users\lucas\Documents\KandidatPyt\FindStats.py</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" t="s">
         <v>106</v>
-      </c>
-      <c r="C15" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4C0ED3-ED2C-4745-9A5F-28E42100EE3D}">
   <dimension ref="B2:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>